<commit_message>
- Refactored MyCoolSearcher such that it can accept all tuning variables - Improved the report slightly - Added a report in a form of PDF file
</commit_message>
<xml_diff>
--- a/StatisticalReport.xlsx
+++ b/StatisticalReport.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="230" documentId="11_F25DC773A252ABEACE02EC59335F47F45BDE589C" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{B99C9A3D-BE5A-4F57-BD7F-DF8F8BFC6E01}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="11_F25DC773A252ABEACE02EC59335F47F45BDE589C" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2B538C31-3228-44A3-9EBC-BABF34B4F9D1}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="9960" windowWidth="14610" windowHeight="15240" tabRatio="413" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="375" windowWidth="29040" windowHeight="15345" tabRatio="413" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
     <sheet name="BM25" sheetId="1" r:id="rId2"/>
     <sheet name="Jaccard" sheetId="2" r:id="rId3"/>
     <sheet name="Tf-Idf" sheetId="3" r:id="rId4"/>
+    <sheet name="Time Consumption" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,6 +27,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+  <si>
+    <t>Jaccard</t>
+  </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>TF-IDF</t>
+  </si>
+  <si>
+    <t>BM25</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>iteration</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -55,12 +79,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1845,6 +1915,1851 @@
           <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
           <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
         </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0">
+                <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>Computation time of Jaccard, TF-IDF and BM25 (30 Iterations)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Time Consumption'!$B$1:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Jaccard</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Time Consumption'!$A$3:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Time Consumption'!$B$3:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>2510</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1879</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1718</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1757</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1836</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1822</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1715</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1769</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1721</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1783</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1719</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1739</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1781</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1825</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1795</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1719</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1769</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1771</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1714</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1754</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1821</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1821</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1804</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1752</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1694</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BD3C-4FF4-BB4E-3EF5BDD6A926}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Time Consumption'!$C$1:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>TF-IDF</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Time Consumption'!$A$3:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Time Consumption'!$C$3:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>787</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>763</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>708</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>848</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>776</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>779</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>780</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BD3C-4FF4-BB4E-3EF5BDD6A926}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Time Consumption'!$D$1:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>BM25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Time Consumption'!$A$3:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Time Consumption'!$D$3:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1094</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>762</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>777</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>806</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>761</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>799</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>786</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>786</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>757</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>763</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>818</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>814</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>833</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>795</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>777</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>788</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>791</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BD3C-4FF4-BB4E-3EF5BDD6A926}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="934469760"/>
+        <c:axId val="986975504"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="934469760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iteration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="986975504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="986975504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (Milliseconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="934469760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="10" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="800" b="1" spc="10" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>Precision Curves of TF-IDF, Jaccard and BM25 Searcher (max K = 50)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14111610454334372"/>
+          <c:y val="3.1746026077807049E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="10" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10143407034049343"/>
+          <c:y val="0.23692065521818598"/>
+          <c:w val="0.85913480449021218"/>
+          <c:h val="0.59269725000173745"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>TF-IDF Time (ms)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Time Consumption'!$C$3:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>787</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>763</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>708</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>848</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>776</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>779</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>780</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-ECDE-458D-953A-071F6AC57946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Jaccard Time (ms)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Time Consumption'!$B$3:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>2510</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1879</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1718</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1757</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1836</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1822</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1715</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1769</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1721</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1783</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1719</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1739</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1781</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1825</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1795</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1719</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1769</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1771</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1714</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1754</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1821</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1821</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1804</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1752</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1694</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-ECDE-458D-953A-071F6AC57946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BM25 Time (ms)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Time Consumption'!$D$3:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1094</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>762</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>777</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>806</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>761</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>799</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>786</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>786</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>757</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>763</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>818</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>814</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>833</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>795</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>777</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>788</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>791</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-ECDE-458D-953A-071F6AC57946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1570671008"/>
+        <c:axId val="1583024448"/>
+        <c:extLst/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1570671008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1">
+                    <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>K</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.48853670635722146"/>
+              <c:y val="0.91906755808215923"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="700" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1583024448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="200"/>
+        <c:tickLblSkip val="5"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1583024448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1570671008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.2586758791412103E-2"/>
+          <c:y val="0.11385701676963812"/>
+          <c:w val="0.89999983841543718"/>
+          <c:h val="7.3340518189416268E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="900"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -13581,6 +15496,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -14412,6 +16407,1038 @@
 </file>
 
 <file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -19457,6 +22484,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A51C4F97-ED8A-42CE-BF4C-66593194CFD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>339651</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>88605</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>369762</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>58184</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E00DBFA3-7C30-435F-9679-D059E3C42540}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -21169,8 +24273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE16FF97-29BF-4D09-82C4-2A9DE10F67FD}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D50"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21879,4 +24983,489 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C33C99-B619-49E7-842C-12DF56DED4DF}">
+  <dimension ref="A1:D35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="129" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2510</v>
+      </c>
+      <c r="C3" s="1">
+        <v>890</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1879</v>
+      </c>
+      <c r="C4" s="1">
+        <v>798</v>
+      </c>
+      <c r="D4" s="1">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1830</v>
+      </c>
+      <c r="C5" s="1">
+        <v>778</v>
+      </c>
+      <c r="D5" s="1">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1718</v>
+      </c>
+      <c r="C6" s="1">
+        <v>789</v>
+      </c>
+      <c r="D6" s="1">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1830</v>
+      </c>
+      <c r="C7" s="1">
+        <v>736</v>
+      </c>
+      <c r="D7" s="1">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1757</v>
+      </c>
+      <c r="C8" s="1">
+        <v>778</v>
+      </c>
+      <c r="D8" s="1">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1830</v>
+      </c>
+      <c r="C9" s="1">
+        <v>800</v>
+      </c>
+      <c r="D9" s="1">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1795</v>
+      </c>
+      <c r="C10" s="1">
+        <v>773</v>
+      </c>
+      <c r="D10" s="1">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1836</v>
+      </c>
+      <c r="C11" s="1">
+        <v>740</v>
+      </c>
+      <c r="D11" s="1">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1822</v>
+      </c>
+      <c r="C12" s="1">
+        <v>789</v>
+      </c>
+      <c r="D12" s="1">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1715</v>
+      </c>
+      <c r="C13" s="1">
+        <v>772</v>
+      </c>
+      <c r="D13" s="1">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1769</v>
+      </c>
+      <c r="C14" s="1">
+        <v>726</v>
+      </c>
+      <c r="D14" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1721</v>
+      </c>
+      <c r="C15" s="1">
+        <v>720</v>
+      </c>
+      <c r="D15" s="1">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1801</v>
+      </c>
+      <c r="C16" s="1">
+        <v>729</v>
+      </c>
+      <c r="D16" s="1">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1783</v>
+      </c>
+      <c r="C17" s="1">
+        <v>787</v>
+      </c>
+      <c r="D17" s="1">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1719</v>
+      </c>
+      <c r="C18" s="1">
+        <v>763</v>
+      </c>
+      <c r="D18" s="1">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1739</v>
+      </c>
+      <c r="C19" s="1">
+        <v>712</v>
+      </c>
+      <c r="D19" s="1">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1781</v>
+      </c>
+      <c r="C20" s="1">
+        <v>721</v>
+      </c>
+      <c r="D20" s="1">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1825</v>
+      </c>
+      <c r="C21" s="1">
+        <v>729</v>
+      </c>
+      <c r="D21" s="1">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1795</v>
+      </c>
+      <c r="C22" s="1">
+        <v>780</v>
+      </c>
+      <c r="D22" s="1">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1719</v>
+      </c>
+      <c r="C23" s="1">
+        <v>708</v>
+      </c>
+      <c r="D23" s="1">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1769</v>
+      </c>
+      <c r="C24" s="1">
+        <v>848</v>
+      </c>
+      <c r="D24" s="1">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1771</v>
+      </c>
+      <c r="C25" s="1">
+        <v>774</v>
+      </c>
+      <c r="D25" s="1">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1714</v>
+      </c>
+      <c r="C26" s="1">
+        <v>726</v>
+      </c>
+      <c r="D26" s="1">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1754</v>
+      </c>
+      <c r="C27" s="1">
+        <v>776</v>
+      </c>
+      <c r="D27" s="1">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1821</v>
+      </c>
+      <c r="C28" s="1">
+        <v>751</v>
+      </c>
+      <c r="D28" s="1">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1821</v>
+      </c>
+      <c r="C29" s="1">
+        <v>735</v>
+      </c>
+      <c r="D29" s="1">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1804</v>
+      </c>
+      <c r="C30" s="1">
+        <v>722</v>
+      </c>
+      <c r="D30" s="1">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1752</v>
+      </c>
+      <c r="C31" s="1">
+        <v>779</v>
+      </c>
+      <c r="D31" s="1">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1694</v>
+      </c>
+      <c r="C32" s="1">
+        <v>780</v>
+      </c>
+      <c r="D32" s="1">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <f>AVERAGE(B3:B32)</f>
+        <v>1802.4666666666667</v>
+      </c>
+      <c r="C35">
+        <f>AVERAGE(C3:C32)</f>
+        <v>763.63333333333333</v>
+      </c>
+      <c r="D35">
+        <f>AVERAGE(D3:D32)</f>
+        <v>793.33333333333337</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>